<commit_message>
add new api and update sql file
</commit_message>
<xml_diff>
--- a/server/file/学生信息导入模板.xlsx
+++ b/server/file/学生信息导入模板.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20372"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20373"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C7EB3F5-5BA7-43BE-A45D-9ED2B53FDDC2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D3BB35E-D644-471C-B742-B15546385B0A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,11 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
-  <si>
-    <t>序号</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="133">
   <si>
     <t>身份证号</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -63,6 +59,387 @@
   </si>
   <si>
     <t>学生姓名</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>学号</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>28</t>
+  </si>
+  <si>
+    <t>29</t>
+  </si>
+  <si>
+    <t>张3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>张4</t>
+  </si>
+  <si>
+    <t>张5</t>
+  </si>
+  <si>
+    <t>张6</t>
+  </si>
+  <si>
+    <t>张7</t>
+  </si>
+  <si>
+    <t>张8</t>
+  </si>
+  <si>
+    <t>张9</t>
+  </si>
+  <si>
+    <t>张10</t>
+  </si>
+  <si>
+    <t>张11</t>
+  </si>
+  <si>
+    <t>张12</t>
+  </si>
+  <si>
+    <t>张13</t>
+  </si>
+  <si>
+    <t>张14</t>
+  </si>
+  <si>
+    <t>张15</t>
+  </si>
+  <si>
+    <t>张16</t>
+  </si>
+  <si>
+    <t>张17</t>
+  </si>
+  <si>
+    <t>张18</t>
+  </si>
+  <si>
+    <t>张19</t>
+  </si>
+  <si>
+    <t>张20</t>
+  </si>
+  <si>
+    <t>张21</t>
+  </si>
+  <si>
+    <t>张22</t>
+  </si>
+  <si>
+    <t>张23</t>
+  </si>
+  <si>
+    <t>张24</t>
+  </si>
+  <si>
+    <t>张25</t>
+  </si>
+  <si>
+    <t>张26</t>
+  </si>
+  <si>
+    <t>张27</t>
+  </si>
+  <si>
+    <t>张28</t>
+  </si>
+  <si>
+    <t>张29</t>
+  </si>
+  <si>
+    <t>张30</t>
+  </si>
+  <si>
+    <t>张31</t>
+  </si>
+  <si>
+    <t>汉</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>男</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>信息</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>计算机</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>北京</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>丝滑</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1112313</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1112314</t>
+  </si>
+  <si>
+    <t>1112315</t>
+  </si>
+  <si>
+    <t>1112316</t>
+  </si>
+  <si>
+    <t>1112317</t>
+  </si>
+  <si>
+    <t>1112318</t>
+  </si>
+  <si>
+    <t>1112319</t>
+  </si>
+  <si>
+    <t>1112320</t>
+  </si>
+  <si>
+    <t>1112321</t>
+  </si>
+  <si>
+    <t>1112322</t>
+  </si>
+  <si>
+    <t>1112323</t>
+  </si>
+  <si>
+    <t>1112324</t>
+  </si>
+  <si>
+    <t>1112325</t>
+  </si>
+  <si>
+    <t>1112326</t>
+  </si>
+  <si>
+    <t>1112327</t>
+  </si>
+  <si>
+    <t>1112328</t>
+  </si>
+  <si>
+    <t>1112329</t>
+  </si>
+  <si>
+    <t>1112330</t>
+  </si>
+  <si>
+    <t>1112331</t>
+  </si>
+  <si>
+    <t>1112332</t>
+  </si>
+  <si>
+    <t>1112333</t>
+  </si>
+  <si>
+    <t>1112334</t>
+  </si>
+  <si>
+    <t>1112335</t>
+  </si>
+  <si>
+    <t>1112336</t>
+  </si>
+  <si>
+    <t>1112337</t>
+  </si>
+  <si>
+    <t>1112338</t>
+  </si>
+  <si>
+    <t>1112339</t>
+  </si>
+  <si>
+    <t>1112340</t>
+  </si>
+  <si>
+    <t>123</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>124</t>
+  </si>
+  <si>
+    <t>125</t>
+  </si>
+  <si>
+    <t>126</t>
+  </si>
+  <si>
+    <t>127</t>
+  </si>
+  <si>
+    <t>128</t>
+  </si>
+  <si>
+    <t>129</t>
+  </si>
+  <si>
+    <t>130</t>
+  </si>
+  <si>
+    <t>131</t>
+  </si>
+  <si>
+    <t>132</t>
+  </si>
+  <si>
+    <t>133</t>
+  </si>
+  <si>
+    <t>134</t>
+  </si>
+  <si>
+    <t>135</t>
+  </si>
+  <si>
+    <t>136</t>
+  </si>
+  <si>
+    <t>137</t>
+  </si>
+  <si>
+    <t>138</t>
+  </si>
+  <si>
+    <t>139</t>
+  </si>
+  <si>
+    <t>140</t>
+  </si>
+  <si>
+    <t>141</t>
+  </si>
+  <si>
+    <t>142</t>
+  </si>
+  <si>
+    <t>143</t>
+  </si>
+  <si>
+    <t>144</t>
+  </si>
+  <si>
+    <t>145</t>
+  </si>
+  <si>
+    <t>146</t>
+  </si>
+  <si>
+    <t>147</t>
+  </si>
+  <si>
+    <t>148</t>
+  </si>
+  <si>
+    <t>149</t>
+  </si>
+  <si>
+    <t>150</t>
+  </si>
+  <si>
+    <t>151</t>
+  </si>
+  <si>
+    <t>12345678900</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -106,8 +483,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -388,47 +766,1068 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K1"/>
+  <dimension ref="A1:K30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+    <sheetView tabSelected="1" topLeftCell="D8" workbookViewId="0">
+      <selection activeCell="L25" sqref="L25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="14.77734375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="13.109375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="13.109375" style="1" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" t="s">
-        <v>9</v>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F2" t="s">
+        <v>71</v>
+      </c>
+      <c r="G2" t="s">
+        <v>72</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="I2" t="s">
+        <v>73</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="K2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E3" t="s">
+        <v>70</v>
+      </c>
+      <c r="F3" t="s">
+        <v>71</v>
+      </c>
+      <c r="G3" t="s">
+        <v>72</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="I3" t="s">
+        <v>73</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="K3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D4" t="s">
+        <v>69</v>
+      </c>
+      <c r="E4" t="s">
+        <v>70</v>
+      </c>
+      <c r="F4" t="s">
+        <v>71</v>
+      </c>
+      <c r="G4" t="s">
+        <v>72</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="I4" t="s">
+        <v>73</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="K4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D5" t="s">
+        <v>69</v>
+      </c>
+      <c r="E5" t="s">
+        <v>70</v>
+      </c>
+      <c r="F5" t="s">
+        <v>71</v>
+      </c>
+      <c r="G5" t="s">
+        <v>72</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="I5" t="s">
+        <v>73</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="K5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D6" t="s">
+        <v>69</v>
+      </c>
+      <c r="E6" t="s">
+        <v>70</v>
+      </c>
+      <c r="F6" t="s">
+        <v>71</v>
+      </c>
+      <c r="G6" t="s">
+        <v>72</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="I6" t="s">
+        <v>73</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="K6" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D7" t="s">
+        <v>69</v>
+      </c>
+      <c r="E7" t="s">
+        <v>70</v>
+      </c>
+      <c r="F7" t="s">
+        <v>71</v>
+      </c>
+      <c r="G7" t="s">
+        <v>72</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="I7" t="s">
+        <v>73</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="K7" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" t="s">
+        <v>46</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D8" t="s">
+        <v>69</v>
+      </c>
+      <c r="E8" t="s">
+        <v>70</v>
+      </c>
+      <c r="F8" t="s">
+        <v>71</v>
+      </c>
+      <c r="G8" t="s">
+        <v>72</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="I8" t="s">
+        <v>73</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="K8" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D9" t="s">
+        <v>69</v>
+      </c>
+      <c r="E9" t="s">
+        <v>70</v>
+      </c>
+      <c r="F9" t="s">
+        <v>71</v>
+      </c>
+      <c r="G9" t="s">
+        <v>72</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="I9" t="s">
+        <v>73</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="K9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" t="s">
+        <v>48</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D10" t="s">
+        <v>69</v>
+      </c>
+      <c r="E10" t="s">
+        <v>70</v>
+      </c>
+      <c r="F10" t="s">
+        <v>71</v>
+      </c>
+      <c r="G10" t="s">
+        <v>72</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="I10" t="s">
+        <v>73</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="K10" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" t="s">
+        <v>49</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D11" t="s">
+        <v>69</v>
+      </c>
+      <c r="E11" t="s">
+        <v>70</v>
+      </c>
+      <c r="F11" t="s">
+        <v>71</v>
+      </c>
+      <c r="G11" t="s">
+        <v>72</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="I11" t="s">
+        <v>73</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="K11" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" t="s">
+        <v>50</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D12" t="s">
+        <v>69</v>
+      </c>
+      <c r="E12" t="s">
+        <v>70</v>
+      </c>
+      <c r="F12" t="s">
+        <v>71</v>
+      </c>
+      <c r="G12" t="s">
+        <v>72</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="I12" t="s">
+        <v>73</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="K12" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" t="s">
+        <v>51</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D13" t="s">
+        <v>69</v>
+      </c>
+      <c r="E13" t="s">
+        <v>70</v>
+      </c>
+      <c r="F13" t="s">
+        <v>71</v>
+      </c>
+      <c r="G13" t="s">
+        <v>72</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="I13" t="s">
+        <v>73</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="K13" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" t="s">
+        <v>52</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="D14" t="s">
+        <v>69</v>
+      </c>
+      <c r="E14" t="s">
+        <v>70</v>
+      </c>
+      <c r="F14" t="s">
+        <v>71</v>
+      </c>
+      <c r="G14" t="s">
+        <v>72</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="I14" t="s">
+        <v>73</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="K14" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" t="s">
+        <v>53</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D15" t="s">
+        <v>69</v>
+      </c>
+      <c r="E15" t="s">
+        <v>70</v>
+      </c>
+      <c r="F15" t="s">
+        <v>71</v>
+      </c>
+      <c r="G15" t="s">
+        <v>72</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="I15" t="s">
+        <v>73</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="K15" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" t="s">
+        <v>54</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D16" t="s">
+        <v>69</v>
+      </c>
+      <c r="E16" t="s">
+        <v>70</v>
+      </c>
+      <c r="F16" t="s">
+        <v>71</v>
+      </c>
+      <c r="G16" t="s">
+        <v>72</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="I16" t="s">
+        <v>73</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="K16" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" t="s">
+        <v>55</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D17" t="s">
+        <v>69</v>
+      </c>
+      <c r="E17" t="s">
+        <v>70</v>
+      </c>
+      <c r="F17" t="s">
+        <v>71</v>
+      </c>
+      <c r="G17" t="s">
+        <v>72</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="I17" t="s">
+        <v>73</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="K17" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" t="s">
+        <v>56</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D18" t="s">
+        <v>69</v>
+      </c>
+      <c r="E18" t="s">
+        <v>70</v>
+      </c>
+      <c r="F18" t="s">
+        <v>71</v>
+      </c>
+      <c r="G18" t="s">
+        <v>72</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="I18" t="s">
+        <v>73</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="K18" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B19" t="s">
+        <v>57</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D19" t="s">
+        <v>69</v>
+      </c>
+      <c r="E19" t="s">
+        <v>70</v>
+      </c>
+      <c r="F19" t="s">
+        <v>71</v>
+      </c>
+      <c r="G19" t="s">
+        <v>72</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="I19" t="s">
+        <v>73</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="K19" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" t="s">
+        <v>58</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="D20" t="s">
+        <v>69</v>
+      </c>
+      <c r="E20" t="s">
+        <v>70</v>
+      </c>
+      <c r="F20" t="s">
+        <v>71</v>
+      </c>
+      <c r="G20" t="s">
+        <v>72</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="I20" t="s">
+        <v>73</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="K20" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B21" t="s">
+        <v>59</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="D21" t="s">
+        <v>69</v>
+      </c>
+      <c r="E21" t="s">
+        <v>70</v>
+      </c>
+      <c r="F21" t="s">
+        <v>71</v>
+      </c>
+      <c r="G21" t="s">
+        <v>72</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="I21" t="s">
+        <v>73</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="K21" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B22" t="s">
+        <v>60</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D22" t="s">
+        <v>69</v>
+      </c>
+      <c r="E22" t="s">
+        <v>70</v>
+      </c>
+      <c r="F22" t="s">
+        <v>71</v>
+      </c>
+      <c r="G22" t="s">
+        <v>72</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="I22" t="s">
+        <v>73</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="K22" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B23" t="s">
+        <v>61</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D23" t="s">
+        <v>69</v>
+      </c>
+      <c r="E23" t="s">
+        <v>70</v>
+      </c>
+      <c r="F23" t="s">
+        <v>71</v>
+      </c>
+      <c r="G23" t="s">
+        <v>72</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="I23" t="s">
+        <v>73</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="K23" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B24" t="s">
+        <v>62</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D24" t="s">
+        <v>69</v>
+      </c>
+      <c r="E24" t="s">
+        <v>70</v>
+      </c>
+      <c r="F24" t="s">
+        <v>71</v>
+      </c>
+      <c r="G24" t="s">
+        <v>72</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="I24" t="s">
+        <v>73</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="K24" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B25" t="s">
+        <v>63</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D25" t="s">
+        <v>69</v>
+      </c>
+      <c r="E25" t="s">
+        <v>70</v>
+      </c>
+      <c r="F25" t="s">
+        <v>71</v>
+      </c>
+      <c r="G25" t="s">
+        <v>72</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="I25" t="s">
+        <v>73</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="K25" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B26" t="s">
+        <v>64</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D26" t="s">
+        <v>69</v>
+      </c>
+      <c r="E26" t="s">
+        <v>70</v>
+      </c>
+      <c r="F26" t="s">
+        <v>71</v>
+      </c>
+      <c r="G26" t="s">
+        <v>72</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="I26" t="s">
+        <v>73</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="K26" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B27" t="s">
+        <v>65</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D27" t="s">
+        <v>69</v>
+      </c>
+      <c r="E27" t="s">
+        <v>70</v>
+      </c>
+      <c r="F27" t="s">
+        <v>71</v>
+      </c>
+      <c r="G27" t="s">
+        <v>72</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="I27" t="s">
+        <v>73</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="K27" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B28" t="s">
+        <v>66</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D28" t="s">
+        <v>69</v>
+      </c>
+      <c r="E28" t="s">
+        <v>70</v>
+      </c>
+      <c r="F28" t="s">
+        <v>71</v>
+      </c>
+      <c r="G28" t="s">
+        <v>72</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="I28" t="s">
+        <v>73</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="K28" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B29" t="s">
+        <v>67</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D29" t="s">
+        <v>69</v>
+      </c>
+      <c r="E29" t="s">
+        <v>70</v>
+      </c>
+      <c r="F29" t="s">
+        <v>71</v>
+      </c>
+      <c r="G29" t="s">
+        <v>72</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="I29" t="s">
+        <v>73</v>
+      </c>
+      <c r="J29" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="K29" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B30" t="s">
+        <v>68</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D30" t="s">
+        <v>69</v>
+      </c>
+      <c r="E30" t="s">
+        <v>70</v>
+      </c>
+      <c r="F30" t="s">
+        <v>71</v>
+      </c>
+      <c r="G30" t="s">
+        <v>72</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="I30" t="s">
+        <v>73</v>
+      </c>
+      <c r="J30" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="K30" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>